<commit_message>
PC serial Price Update 11,13,14,15
</commit_message>
<xml_diff>
--- a/GTL IT Equipment Information 22 Jan 2026.xlsx
+++ b/GTL IT Equipment Information 22 Jan 2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C3FBA3-5186-4556-90B8-117047A21179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4332D5-509C-47DA-A8DB-E7B0A9E7D828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{001EF0C8-142C-468E-BF1A-4ED3A51EB992}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{001EF0C8-142C-468E-BF1A-4ED3A51EB992}"/>
   </bookViews>
   <sheets>
     <sheet name="Laptop" sheetId="9" r:id="rId1"/>
@@ -1118,6 +1118,12 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1141,12 +1147,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,9 +1464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9563A678-2561-40B9-80A5-83AF2D201A32}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V15" sqref="V15"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,7 +2248,7 @@
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="51" t="s">
         <v>144</v>
       </c>
       <c r="B22" s="27">
@@ -2290,7 +2290,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="60"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="45">
         <v>19</v>
       </c>
@@ -2923,9 +2923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF07E723-A545-457F-A8A3-D73EE92F41F2}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2946,38 +2946,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="58"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3622,7 +3622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3639,28 +3639,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4100,18 +4100,18 @@
       <c r="O1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4444,18 +4444,18 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -4555,14 +4555,14 @@
       <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
PC Data Update of 13,14
</commit_message>
<xml_diff>
--- a/GTL IT Equipment Information 22 Jan 2026.xlsx
+++ b/GTL IT Equipment Information 22 Jan 2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4332D5-509C-47DA-A8DB-E7B0A9E7D828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB80D53D-0A7D-4527-97C5-26C531E15952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{001EF0C8-142C-468E-BF1A-4ED3A51EB992}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="241">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>15s-Fq5317TU</t>
+  </si>
+  <si>
+    <t>Dual Core</t>
   </si>
 </sst>
 </file>
@@ -2925,7 +2928,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3521,10 +3524,18 @@
       <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="9"/>
+      <c r="D17" s="17">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="17">
+        <v>256</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
         <v>49</v>
@@ -3550,10 +3561,18 @@
       <c r="C18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="9"/>
+      <c r="D18" s="17">
+        <v>4</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F18" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G18" s="9">
+        <v>3</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Reciption Monitor is Damage
</commit_message>
<xml_diff>
--- a/GTL IT Equipment Information 22 Jan 2026.xlsx
+++ b/GTL IT Equipment Information 22 Jan 2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB80D53D-0A7D-4527-97C5-26C531E15952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA835C6-A185-4600-91B0-7FEBB6D5EAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{001EF0C8-142C-468E-BF1A-4ED3A51EB992}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{001EF0C8-142C-468E-BF1A-4ED3A51EB992}"/>
   </bookViews>
   <sheets>
     <sheet name="Laptop" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="238">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -133,9 +133,6 @@
     <t>3rd Floor</t>
   </si>
   <si>
-    <t>8th Floor</t>
-  </si>
-  <si>
     <t>Clone PC</t>
   </si>
   <si>
@@ -169,13 +166,7 @@
     <t>Dell Monitor</t>
   </si>
   <si>
-    <t>E170SC</t>
-  </si>
-  <si>
     <t>IT Room</t>
-  </si>
-  <si>
-    <t>Reception</t>
   </si>
   <si>
     <t>Management Room</t>
@@ -1468,7 +1459,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
@@ -1510,7 +1501,7 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -1572,22 +1563,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B4" s="27">
         <v>1</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E4" s="27">
         <v>8</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G4" s="27">
         <v>500</v>
@@ -1597,7 +1588,7 @@
       </c>
       <c r="I4" s="27"/>
       <c r="J4" s="32" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K4" s="27" t="s">
         <v>8</v>
@@ -1616,16 +1607,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E5" s="27">
         <v>8</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G5" s="27">
         <v>500</v>
@@ -1635,10 +1626,10 @@
       </c>
       <c r="I5" s="27"/>
       <c r="J5" s="32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>19</v>
@@ -1650,16 +1641,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B6" s="8">
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E6" s="8">
         <v>8</v>
@@ -1675,7 +1666,7 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="30" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>8</v>
@@ -1694,10 +1685,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E7" s="8">
         <v>8</v>
@@ -1713,10 +1704,10 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>17</v>
@@ -1732,10 +1723,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E8" s="31">
         <v>8</v>
@@ -1750,10 +1741,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>8</v>
@@ -1772,10 +1763,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E9" s="8">
         <v>8</v>
@@ -1790,10 +1781,10 @@
         <v>11</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>8</v>
@@ -1812,10 +1803,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E10" s="8">
         <v>8</v>
@@ -1831,10 +1822,10 @@
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>19</v>
@@ -1850,10 +1841,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E11" s="8">
         <v>8</v>
@@ -1869,10 +1860,10 @@
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>19</v>
@@ -1888,10 +1879,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E12" s="8">
         <v>8</v>
@@ -1907,10 +1898,10 @@
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>19</v>
@@ -1926,10 +1917,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E13" s="8">
         <v>8</v>
@@ -1944,10 +1935,10 @@
         <v>11</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>8</v>
@@ -1966,10 +1957,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E14" s="8">
         <v>8</v>
@@ -1984,10 +1975,10 @@
         <v>11</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>8</v>
@@ -2006,10 +1997,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E15" s="8">
         <v>4</v>
@@ -2024,20 +2015,20 @@
         <v>10</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2046,10 +2037,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E16" s="8">
         <v>8</v>
@@ -2065,31 +2056,31 @@
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="30" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B17" s="7">
         <v>14</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E17" s="7">
         <v>4</v>
@@ -2098,17 +2089,17 @@
         <v>9</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H17" s="7">
         <v>11</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>19</v>
@@ -2124,10 +2115,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E18" s="7">
         <v>4</v>
@@ -2143,7 +2134,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>8</v>
@@ -2162,10 +2153,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E19" s="7">
         <v>4</v>
@@ -2181,7 +2172,7 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>8</v>
@@ -2200,10 +2191,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E20" s="7">
         <v>4</v>
@@ -2219,22 +2210,22 @@
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M20" s="6"/>
       <c r="N20" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -2252,22 +2243,22 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B22" s="27">
         <v>18</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E22" s="27">
         <v>8</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G22" s="27">
         <v>240</v>
@@ -2276,10 +2267,10 @@
         <v>7</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J22" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K22" s="27" t="s">
         <v>8</v>
@@ -2298,16 +2289,16 @@
         <v>19</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E23" s="45">
         <v>8</v>
       </c>
       <c r="F23" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>11</v>
@@ -2317,31 +2308,31 @@
       </c>
       <c r="I23" s="45"/>
       <c r="J23" s="32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K23" s="45" t="s">
         <v>8</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B24" s="8">
         <v>20</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E24" s="8">
         <v>7</v>
@@ -2357,7 +2348,7 @@
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>8</v>
@@ -2376,10 +2367,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E25" s="8">
         <v>4</v>
@@ -2395,7 +2386,7 @@
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>8</v>
@@ -2414,10 +2405,10 @@
         <v>22</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E26" s="8">
         <v>8</v>
@@ -2432,10 +2423,10 @@
         <v>8</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>8</v>
@@ -2454,7 +2445,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="8">
@@ -2468,13 +2459,13 @@
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>19</v>
@@ -2490,10 +2481,10 @@
         <v>24</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E28" s="8">
         <v>8</v>
@@ -2509,7 +2500,7 @@
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>8</v>
@@ -2528,10 +2519,10 @@
         <v>25</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E29" s="8">
         <v>8</v>
@@ -2547,7 +2538,7 @@
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>8</v>
@@ -2566,10 +2557,10 @@
         <v>26</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E30" s="8">
         <v>8</v>
@@ -2584,10 +2575,10 @@
         <v>7</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>8</v>
@@ -2606,10 +2597,10 @@
         <v>27</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E31" s="8">
         <v>4</v>
@@ -2625,17 +2616,17 @@
       </c>
       <c r="I31" s="8"/>
       <c r="J31" s="26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M31" s="6"/>
       <c r="N31" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2644,10 +2635,10 @@
         <v>28</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E32" s="8">
         <v>4</v>
@@ -2663,17 +2654,17 @@
       </c>
       <c r="I32" s="8"/>
       <c r="J32" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K32" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M32" s="6"/>
       <c r="N32" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2682,10 +2673,10 @@
         <v>29</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E33" s="8">
         <v>4</v>
@@ -2701,17 +2692,17 @@
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M33" s="6"/>
       <c r="N33" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -2720,10 +2711,10 @@
         <v>30</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E34" s="8">
         <v>4</v>
@@ -2739,31 +2730,31 @@
       </c>
       <c r="I34" s="8"/>
       <c r="J34" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K34" s="44" t="s">
         <v>8</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M34" s="6"/>
       <c r="N34" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B35" s="7">
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>117</v>
       </c>
       <c r="E35" s="7">
         <v>4</v>
@@ -2778,20 +2769,20 @@
         <v>5</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M35" s="6"/>
       <c r="N35" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -2800,10 +2791,10 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E36" s="7">
         <v>4</v>
@@ -2819,17 +2810,17 @@
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M36" s="6"/>
       <c r="N36" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -2838,10 +2829,10 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E37" s="7">
         <v>4</v>
@@ -2857,17 +2848,17 @@
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M37" s="6"/>
       <c r="N37" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -2876,7 +2867,7 @@
         <v>34</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7">
@@ -2893,17 +2884,17 @@
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M38" s="6"/>
       <c r="N38" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2926,9 +2917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF07E723-A545-457F-A8A3-D73EE92F41F2}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,7 +2958,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -3028,29 +3019,29 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4">
         <v>32</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G4" s="4">
         <v>4</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>17</v>
@@ -3068,7 +3059,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="17">
         <v>16</v>
@@ -3086,7 +3077,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>33</v>
@@ -3107,7 +3098,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="17">
         <v>16</v>
@@ -3146,7 +3137,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="17">
         <v>16</v>
@@ -3179,13 +3170,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="17">
         <v>16</v>
@@ -3218,13 +3209,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="17">
         <v>16</v>
@@ -3242,7 +3233,7 @@
         <v>25</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>32</v>
@@ -3257,13 +3248,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="17">
         <v>8</v>
@@ -3294,13 +3285,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="17">
         <v>8</v>
@@ -3331,13 +3322,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="17">
         <v>8</v>
@@ -3368,13 +3359,13 @@
     </row>
     <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="17">
         <v>32</v>
@@ -3383,14 +3374,14 @@
         <v>23</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="9">
         <v>11</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J13" s="15" t="s">
         <v>32</v>
@@ -3405,13 +3396,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="17">
         <v>8</v>
@@ -3427,7 +3418,7 @@
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>32</v>
@@ -3442,13 +3433,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="17">
         <v>4</v>
@@ -3464,28 +3455,28 @@
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>32</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D16" s="17">
         <v>8</v>
@@ -3501,28 +3492,28 @@
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="17">
         <v>4</v>
@@ -3538,34 +3529,34 @@
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>32</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="17">
         <v>4</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F18" s="17">
         <v>1000</v>
@@ -3575,28 +3566,28 @@
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>32</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D19" s="17">
         <v>8</v>
@@ -3612,17 +3603,17 @@
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J19" s="15" t="s">
         <v>33</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3637,11 +3628,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1200A48-073D-46CA-B54F-F664BE4B754F}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,7 +3662,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -3698,7 +3689,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
@@ -3712,13 +3703,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>32</v>
@@ -3736,13 +3727,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>32</v>
@@ -3760,13 +3751,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>32</v>
@@ -3784,10 +3775,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>26</v>
@@ -3808,10 +3799,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>27</v>
@@ -3832,16 +3823,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
@@ -3856,13 +3847,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>32</v>
@@ -3880,10 +3871,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>31</v>
@@ -3904,10 +3895,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>31</v>
@@ -3928,10 +3919,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>31</v>
@@ -3952,16 +3943,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>19</v>
@@ -3976,10 +3967,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>29</v>
@@ -4000,19 +3991,19 @@
         <v>13</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="4" t="s">
@@ -4024,46 +4015,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>45</v>
+        <v>190</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>46</v>
+        <v>232</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>48</v>
+        <v>233</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <v>15</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4082,7 +4049,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4120,7 +4087,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -4140,22 +4107,22 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
@@ -4166,25 +4133,25 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>17</v>
@@ -4196,25 +4163,25 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B5" s="27">
         <v>2</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>19</v>
@@ -4226,28 +4193,28 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B6" s="39">
         <v>3</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="4" t="s">
@@ -4256,28 +4223,28 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B7" s="7">
         <v>4</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="4" t="s">
@@ -4286,28 +4253,28 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B8" s="7">
         <v>5</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
@@ -4316,28 +4283,28 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B9" s="37">
         <v>6</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
@@ -4346,28 +4313,28 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B10" s="37">
         <v>7</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
@@ -4376,28 +4343,28 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B11" s="8">
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
@@ -4406,28 +4373,28 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B12" s="8">
         <v>9</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
@@ -4436,26 +4403,26 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B13" s="43">
         <v>10</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
@@ -4464,7 +4431,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -4478,25 +4445,25 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B15" s="35">
         <v>11</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>17</v>
@@ -4508,25 +4475,25 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B16" s="35">
         <v>12</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>17</v>
@@ -4552,7 +4519,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4575,7 +4542,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
@@ -4585,10 +4552,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -4608,10 +4575,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="5"/>
@@ -4624,10 +4591,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="5"/>
@@ -4640,13 +4607,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="4" t="s">
@@ -4658,13 +4625,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="4" t="s">
@@ -4676,13 +4643,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="4" t="s">
@@ -4694,13 +4661,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4" t="s">
@@ -4712,10 +4679,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="5"/>
@@ -4728,13 +4695,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="4" t="s">
@@ -4746,13 +4713,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="4" t="s">
@@ -4764,10 +4731,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -4780,10 +4747,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="5"/>
@@ -4796,13 +4763,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="4" t="s">
@@ -4814,10 +4781,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="5"/>
@@ -4830,7 +4797,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -4839,7 +4806,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>